<commit_message>
Cambio de ultimo minuto: Reporte de ceses
</commit_message>
<xml_diff>
--- a/2-PERSONAL/2-CESES/JUNIO-2022-CESES-PUCUSANA.xlsx
+++ b/2-PERSONAL/2-CESES/JUNIO-2022-CESES-PUCUSANA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AKM\2-PERSONAL\2-CESES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F85BD0F-FA9C-446C-8D89-61E2A8692B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DE9253-3BE0-47E4-A892-CCCCBFA0C244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{07747DA7-88DF-43B8-A3F2-BA3A9EBFFB3D}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="PAGO QUINCENA" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CESES!$A$4:$N$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CESES!$A$4:$N$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
   <si>
     <t>APELLIDOS Y NOMBRES</t>
   </si>
@@ -181,6 +181,48 @@
   </si>
   <si>
     <t>70903536</t>
+  </si>
+  <si>
+    <t>ASTETE MALASQUEZ</t>
+  </si>
+  <si>
+    <t>VICTOR NICOLAS</t>
+  </si>
+  <si>
+    <t>CUYA CHAMORRO</t>
+  </si>
+  <si>
+    <t>BRISA DANA</t>
+  </si>
+  <si>
+    <t>ESPINOZA SANCHEZ</t>
+  </si>
+  <si>
+    <t>JHOEL CRISTHIAN</t>
+  </si>
+  <si>
+    <t>GUTIERREZ LA ROSA</t>
+  </si>
+  <si>
+    <t>KATLEHEN DANIELA</t>
+  </si>
+  <si>
+    <t>ASTETE MALASQUEZ VICTOR NICOLAS</t>
+  </si>
+  <si>
+    <t>CUYA CHAMORRO BRISA DANA</t>
+  </si>
+  <si>
+    <t>ESPINOZA SANCHEZ JHOEL CRISTHIAN</t>
+  </si>
+  <si>
+    <t>71402573</t>
+  </si>
+  <si>
+    <t>60638954</t>
+  </si>
+  <si>
+    <t>73690505</t>
   </si>
 </sst>
 </file>
@@ -655,10 +697,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5DAD48-3949-4D57-8093-C7F1715EEE30}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A2:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>1</v>
       </c>
@@ -757,7 +800,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>2</v>
       </c>
@@ -789,7 +832,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>3</v>
       </c>
@@ -823,7 +866,7 @@
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>4</v>
       </c>
@@ -857,7 +900,7 @@
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>5</v>
       </c>
@@ -889,7 +932,7 @@
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>6</v>
       </c>
@@ -922,15 +965,33 @@
       <c r="N10" s="9"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="3"/>
+      <c r="A11" s="15">
+        <v>7</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="18">
+        <v>44723</v>
+      </c>
+      <c r="E11" s="18">
+        <v>44727</v>
+      </c>
+      <c r="F11" s="18">
+        <v>44734</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="J11" s="3"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
@@ -938,14 +999,30 @@
       <c r="N11" s="9"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+      <c r="A12" s="15">
+        <v>8</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="18">
+        <v>44698</v>
+      </c>
+      <c r="E12" s="18">
+        <v>44730</v>
+      </c>
+      <c r="F12" s="18">
+        <v>44734</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>4</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="9"/>
@@ -954,15 +1031,33 @@
       <c r="N12" s="9"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="3"/>
+      <c r="A13" s="15">
+        <v>9</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="18">
+        <v>44667</v>
+      </c>
+      <c r="E13" s="18">
+        <v>44725</v>
+      </c>
+      <c r="F13" s="18">
+        <v>44734</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="J13" s="3"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
@@ -970,15 +1065,33 @@
       <c r="N13" s="9"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="3"/>
+      <c r="A14" s="15">
+        <v>10</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="18">
+        <v>44644</v>
+      </c>
+      <c r="E14" s="18">
+        <v>44729</v>
+      </c>
+      <c r="F14" s="18">
+        <v>44734</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="J14" s="3"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
@@ -1137,6 +1250,13 @@
       <c r="I25" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A4:N14" xr:uid="{CB5DAD48-3949-4D57-8093-C7F1715EEE30}">
+    <filterColumn colId="5">
+      <filters>
+        <dateGroupItem year="2022" month="6" day="22" dateTimeGrouping="day"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1147,7 +1267,7 @@
   <dimension ref="B4:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B16" sqref="B16:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,34 +1400,50 @@
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+        <v>ASTETE MALASQUEZ VICTOR NICOLAS</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+        <v>CUYA CHAMORRO BRISA DANA</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+        <v>ESPINOZA SANCHEZ JHOEL CRISTHIAN</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+        <v>GUTIERREZ LA ROSA KATLEHEN DANIELA</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="str">

</xml_diff>